<commit_message>
Switch to Gurobi in Markov
</commit_message>
<xml_diff>
--- a/data/NREL-118 7 clusters/Global_Parameters.xlsx
+++ b/data/NREL-118 7 clusters/Global_Parameters.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FelixAuer\Git\LEGO-Pyomo\data\NREL-118\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FelixAuer\Git\LEGO-Pyomo\data\NREL-118 7 clusters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6D4F58A-4C78-4541-9592-AF6061DB65CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B56E4944-A706-43FD-AF32-4645F61951C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="851" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="50190" yWindow="-21810" windowWidth="38640" windowHeight="21120" tabRatio="851" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Global Parameters" sheetId="121" r:id="rId1"/>
@@ -138,9 +138,6 @@
     <t>pSolver</t>
   </si>
   <si>
-    <t>highs</t>
-  </si>
-  <si>
     <t>Selected solver</t>
   </si>
   <si>
@@ -190,6 +187,9 @@
   </si>
   <si>
     <t>No</t>
+  </si>
+  <si>
+    <t>gurobi</t>
   </si>
 </sst>
 </file>
@@ -861,19 +861,19 @@
         <v>23</v>
       </c>
       <c r="C5" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="E5" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="E5" s="11" t="s">
+      <c r="F5" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="F5" s="11" t="s">
+      <c r="G5" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="G5" s="15" t="s">
+      <c r="H5" s="13" t="s">
         <v>27</v>
-      </c>
-      <c r="H5" s="13" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="6" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -897,7 +897,7 @@
         <v>12</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E8" s="11" t="s">
         <v>9</v>
@@ -919,7 +919,7 @@
     </row>
     <row r="10" spans="2:8" s="4" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C10" s="10"/>
       <c r="E10" s="10"/>
@@ -929,10 +929,10 @@
     </row>
     <row r="11" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E11" s="11"/>
       <c r="F11" s="11"/>
@@ -941,19 +941,19 @@
     </row>
     <row r="12" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C12" s="9">
         <v>1E-3</v>
       </c>
       <c r="E12" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="F12" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="G12" s="15" t="s">
         <v>33</v>
-      </c>
-      <c r="F12" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="G12" s="15" t="s">
-        <v>34</v>
       </c>
       <c r="H12" s="13">
         <v>1E-3</v>
@@ -966,10 +966,10 @@
     </row>
     <row r="14" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E14" s="11"/>
       <c r="F14" s="11"/>
@@ -977,19 +977,19 @@
     </row>
     <row r="15" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C15" s="9">
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="E15" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="F15" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="F15" s="11" t="s">
-        <v>39</v>
-      </c>
       <c r="G15" s="15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H15" s="13">
         <v>1E-3</v>
@@ -1090,6 +1090,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101004934E3CB1C58BA43BC6E229E2BF20201" ma:contentTypeVersion="4" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="e33ccc94e63df24f58cb47229b46e190">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="87003a75-b64f-4b22-bf19-aa30740e3d46" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0f0f7a5bb162b669de9ce8ff8278c29f" ns2:_="">
     <xsd:import namespace="87003a75-b64f-4b22-bf19-aa30740e3d46"/>
@@ -1235,35 +1250,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{773946F7-566C-458F-95C9-79B0CCE20E87}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13778B2C-CE05-4B32-8196-2F381FEAC95A}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="87003a75-b64f-4b22-bf19-aa30740e3d46"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1285,9 +1275,19 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13778B2C-CE05-4B32-8196-2F381FEAC95A}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{773946F7-566C-458F-95C9-79B0CCE20E87}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="87003a75-b64f-4b22-bf19-aa30740e3d46"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>